<commit_message>
Correct last exercise and have done the " to be" model
</commit_message>
<xml_diff>
--- a/BA_03/src/ex00_DVR_asis.xlsx
+++ b/BA_03/src/ex00_DVR_asis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Пользователь\Desktop\Business-and-system-analyses\BA_03\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCFD1D2-478D-4F92-AB37-BA15DB2FEC12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DD382F-011B-4BBA-9021-2EBC0CBB5BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
   <si>
     <t>Идентификатор</t>
   </si>
@@ -135,12 +135,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>Отсутствие товара</t>
-  </si>
-  <si>
-    <t>Проблема с работой приложения</t>
-  </si>
-  <si>
     <t>Выбор продукта</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
   </si>
   <si>
     <t>Оформление доставки</t>
-  </si>
-  <si>
-    <t>Отсутсвие товара</t>
   </si>
   <si>
     <t>Отслеживание эффективности
@@ -160,10 +151,6 @@
     <t>"+/-"</t>
   </si>
   <si>
-    <t>Просмотр статистики в приложении
- может быть не предусмотрен</t>
-  </si>
-  <si>
     <t>Выбор заказа из возможных</t>
   </si>
   <si>
@@ -173,55 +160,108 @@
     <t>Доставка заказа</t>
   </si>
   <si>
-    <t>Проблема с блокированием заказа в 
-базе данных</t>
-  </si>
-  <si>
     <t>ввод данных о заказах</t>
   </si>
   <si>
+    <t>Назначение заказа курьеру</t>
+  </si>
+  <si>
+    <t>Контроль выполнения</t>
+  </si>
+  <si>
+    <t>Отмена заказа курьеру</t>
+  </si>
+  <si>
+    <t>Учет движений материалов внутри компании</t>
+  </si>
+  <si>
+    <t>Назначение прав доступа</t>
+  </si>
+  <si>
+    <t>Отмена прав доступа</t>
+  </si>
+  <si>
+    <t>Проверки налогового учета</t>
+  </si>
+  <si>
+    <t>Некорректно отправленые данные бухгалтеру</t>
+  </si>
+  <si>
+    <t>Разработка приложения</t>
+  </si>
+  <si>
+    <t>Внедрение "ищейки"</t>
+  </si>
+  <si>
+    <t>Атака на базу</t>
+  </si>
+  <si>
+    <t>Решение проблемы/позитивный эффект</t>
+  </si>
+  <si>
+    <t>to be</t>
+  </si>
+  <si>
+    <t>Отсутствие агрегации в одном приложении</t>
+  </si>
+  <si>
+    <t>Отстутствие полного списка готовых заказов</t>
+  </si>
+  <si>
     <t>Большой поток заказов, которые 
-тфжело обработать</t>
-  </si>
-  <si>
-    <t>Назначение заказа курьеру</t>
-  </si>
-  <si>
-    <t>Контроль выполнения</t>
-  </si>
-  <si>
-    <t>Отмена заказа курьеру</t>
-  </si>
-  <si>
-    <t>Проблема с работой приложения
-и большой поток заказов</t>
-  </si>
-  <si>
-    <t>Учет движений материалов внутри компании</t>
-  </si>
-  <si>
-    <t>Назначение прав доступа</t>
-  </si>
-  <si>
-    <t>Отмена прав доступа</t>
-  </si>
-  <si>
-    <t>Проверки налогового учета</t>
-  </si>
-  <si>
-    <t>Некорректно отправленые данные бухгалтеру</t>
-  </si>
-  <si>
-    <t>Разработка приложения</t>
-  </si>
-  <si>
-    <t>Внедрение "ищейки"</t>
-  </si>
-  <si>
-    <t>Атака на базу</t>
-  </si>
-  <si>
-    <t>Защита внутри приложения</t>
+тяжело обработать</t>
+  </si>
+  <si>
+    <t>Большой объем заказов</t>
+  </si>
+  <si>
+    <t>Накопление огромного кол-ва документов</t>
+  </si>
+  <si>
+    <t>Когда ничего нет, то и нападать не на что</t>
+  </si>
+  <si>
+    <t>в приложении</t>
+  </si>
+  <si>
+    <t>Проблемы с прогнозированием закупки новых
+ партий продукции</t>
+  </si>
+  <si>
+    <t>Удобный сбор аналитики в одном приложении</t>
+  </si>
+  <si>
+    <t>Не понятно в наличии товар или нет</t>
+  </si>
+  <si>
+    <t>Все будет в одном приложении</t>
+  </si>
+  <si>
+    <t>Все можно будет сделать в телефоне и никуда 
+не выходить</t>
+  </si>
+  <si>
+    <t>Можно будет подключить сервис по типу Grafana,
+ и формировать статистические дашборды</t>
+  </si>
+  <si>
+    <t>Простота и удобство в выборе</t>
+  </si>
+  <si>
+    <t>После бронирования приложение зафиксирует
+заказ и другой курьер не сможет его выполнить одновременно</t>
+  </si>
+  <si>
+    <t>Внутри приложения все можно будет делать автоматизированно</t>
+  </si>
+  <si>
+    <t>Возможность онлайн отправки сделок купли продажи</t>
+  </si>
+  <si>
+    <t>Все данные будут в онлайн формате, уменьшаетс яриск утери</t>
+  </si>
+  <si>
+    <t>Появляется риск падения приложения</t>
   </si>
 </sst>
 </file>
@@ -237,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,8 +296,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -317,11 +363,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -330,12 +385,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -343,14 +392,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,40 +712,58 @@
     <col min="3" max="3" width="41.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="G1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2" s="15"/>
+      <c r="G2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -694,15 +779,31 @@
       <c r="E3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -710,71 +811,119 @@
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -782,210 +931,371 @@
         <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="C18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="10" t="s">
+      <c r="C19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="18"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" s="6" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="18"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="1:6" s="6" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="10" t="s">
+      <c r="C28" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
@@ -993,7 +1303,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>32</v>
@@ -1002,9 +1312,25 @@
         <v>32</v>
       </c>
       <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" s="6" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
@@ -1012,7 +1338,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>32</v>
@@ -1022,6 +1348,15 @@
       </c>
       <c r="F32" s="4" t="s">
         <v>61</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1153,7 +1488,10 @@
       <c r="B110" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="I17:I19"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
Make ex03 and 04
</commit_message>
<xml_diff>
--- a/BA_03/src/ex00_DVR_asis.xlsx
+++ b/BA_03/src/ex00_DVR_asis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Пользователь\Desktop\Business-and-system-analyses\BA_03\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DD382F-011B-4BBA-9021-2EBC0CBB5BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15247EF3-227C-4F3F-B367-ECEFB3651531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <t>Идентификатор</t>
   </si>
@@ -196,12 +196,6 @@
     <t>Атака на базу</t>
   </si>
   <si>
-    <t>Решение проблемы/позитивный эффект</t>
-  </si>
-  <si>
-    <t>to be</t>
-  </si>
-  <si>
     <t>Отсутствие агрегации в одном приложении</t>
   </si>
   <si>
@@ -221,47 +215,11 @@
     <t>Когда ничего нет, то и нападать не на что</t>
   </si>
   <si>
-    <t>в приложении</t>
-  </si>
-  <si>
     <t>Проблемы с прогнозированием закупки новых
  партий продукции</t>
   </si>
   <si>
-    <t>Удобный сбор аналитики в одном приложении</t>
-  </si>
-  <si>
     <t>Не понятно в наличии товар или нет</t>
-  </si>
-  <si>
-    <t>Все будет в одном приложении</t>
-  </si>
-  <si>
-    <t>Все можно будет сделать в телефоне и никуда 
-не выходить</t>
-  </si>
-  <si>
-    <t>Можно будет подключить сервис по типу Grafana,
- и формировать статистические дашборды</t>
-  </si>
-  <si>
-    <t>Простота и удобство в выборе</t>
-  </si>
-  <si>
-    <t>После бронирования приложение зафиксирует
-заказ и другой курьер не сможет его выполнить одновременно</t>
-  </si>
-  <si>
-    <t>Внутри приложения все можно будет делать автоматизированно</t>
-  </si>
-  <si>
-    <t>Возможность онлайн отправки сделок купли продажи</t>
-  </si>
-  <si>
-    <t>Все данные будут в онлайн формате, уменьшаетс яриск утери</t>
-  </si>
-  <si>
-    <t>Появляется риск падения приложения</t>
   </si>
 </sst>
 </file>
@@ -277,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,14 +254,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -363,20 +315,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -392,6 +335,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -403,21 +350,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,57 +645,40 @@
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="58.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="16"/>
+    <col min="7" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:6" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -780,30 +695,18 @@
         <v>33</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="7"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="18"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -818,19 +721,10 @@
         <v>33</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -840,18 +734,9 @@
       <c r="E6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -861,29 +746,17 @@
       <c r="E7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -900,30 +773,18 @@
         <v>33</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -940,19 +801,10 @@
         <v>32</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -965,17 +817,8 @@
         <v>32</v>
       </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -988,25 +831,16 @@
         <v>33</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="18"/>
-    </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1023,27 +857,18 @@
         <v>33</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="18"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -1059,20 +884,11 @@
       <c r="E17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F17" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8" t="s">
@@ -1084,16 +900,9 @@
       <c r="E18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="17"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8" t="s">
@@ -1105,27 +914,17 @@
       <c r="E19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="17"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="18"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
@@ -1142,30 +941,18 @@
         <v>33</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="18"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -1182,14 +969,8 @@
         <v>32</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8" t="s">
@@ -1202,25 +983,16 @@
         <v>32</v>
       </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1239,28 +1011,16 @@
       <c r="F26" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" s="19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
@@ -1277,25 +1037,16 @@
         <v>33</v>
       </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="18"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
@@ -1312,25 +1063,16 @@
         <v>32</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="18"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
@@ -1347,16 +1089,7 @@
         <v>32</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I32" s="19" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1488,17 +1221,14 @@
       <c r="B110" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F17:F19"/>
+  <mergeCells count="7">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F17:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>